<commit_message>
opdateret realiseret tidsplan samt processrapport logbog for dagens arbejde.
</commit_message>
<xml_diff>
--- a/Assets/Documents/Realiseret_tidsplan.xlsx
+++ b/Assets/Documents/Realiseret_tidsplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\92agg\Desktop\Svendeprøve\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CD690C-589D-4CFE-9ED4-ACB64DFB43F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C53928-900A-4ED6-B745-7174A4B860FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5910" yWindow="1770" windowWidth="21600" windowHeight="11295" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -347,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -425,6 +425,15 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -434,13 +443,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -764,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0E67C9-148C-445C-AEDA-6C5F365E02ED}">
   <dimension ref="B1:AB61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,13 +783,13 @@
   <sheetData>
     <row r="1" spans="2:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -795,14 +801,14 @@
     </row>
     <row r="3" spans="2:28" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="29">
+      <c r="C4" s="31"/>
+      <c r="D4" s="32">
         <v>45391</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="2:28" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:28" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -959,7 +965,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="30"/>
+      <c r="I10" s="27"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1058,7 +1064,7 @@
       <c r="U13" s="23"/>
       <c r="V13" s="23"/>
       <c r="W13" s="23"/>
-      <c r="X13" s="31"/>
+      <c r="X13" s="28"/>
       <c r="Z13" s="9"/>
       <c r="AB13" s="4" t="s">
         <v>4</v>
@@ -1102,7 +1108,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
-      <c r="I15" s="32"/>
+      <c r="I15" s="29"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
@@ -1131,7 +1137,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
+      <c r="J16" s="29"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -1159,7 +1165,7 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+      <c r="J17" s="29"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -1329,8 +1335,8 @@
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
@@ -1401,8 +1407,8 @@
       <c r="F27" s="23"/>
       <c r="G27" s="23"/>
       <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
       <c r="K27" s="23"/>
       <c r="L27" s="23"/>
       <c r="M27" s="23"/>
@@ -1452,9 +1458,9 @@
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
@@ -1476,7 +1482,7 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
+      <c r="I30" s="34"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
@@ -1501,7 +1507,7 @@
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
+      <c r="J31" s="34"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
@@ -1525,7 +1531,7 @@
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
+      <c r="J32" s="34"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
@@ -1549,7 +1555,7 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
+      <c r="J33" s="34"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
@@ -1573,7 +1579,7 @@
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
+      <c r="J34" s="34"/>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
@@ -1598,7 +1604,7 @@
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
+      <c r="K35" s="34"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
@@ -1622,7 +1628,7 @@
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
+      <c r="K36" s="34"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>

</xml_diff>

<commit_message>
opdatering af realiseret tidsplan for dagens arbejde
</commit_message>
<xml_diff>
--- a/Assets/Documents/Realiseret_tidsplan.xlsx
+++ b/Assets/Documents/Realiseret_tidsplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\92agg\Desktop\Svendeprøve\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C53928-900A-4ED6-B745-7174A4B860FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479E0262-1B9D-416C-AEF4-B878ABED3EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
+    <workbookView xWindow="-16320" yWindow="-7260" windowWidth="16440" windowHeight="28320" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -434,6 +434,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -442,12 +448,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0E67C9-148C-445C-AEDA-6C5F365E02ED}">
   <dimension ref="B1:AB61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,13 +783,13 @@
   <sheetData>
     <row r="1" spans="2:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -801,14 +801,14 @@
     </row>
     <row r="3" spans="2:28" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32">
+      <c r="C4" s="33"/>
+      <c r="D4" s="34">
         <v>45391</v>
       </c>
-      <c r="E4" s="32"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="2:28" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:28" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -909,7 +909,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="5"/>
+      <c r="I8" s="12"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1335,8 +1335,8 @@
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
@@ -1407,8 +1407,8 @@
       <c r="F27" s="23"/>
       <c r="G27" s="23"/>
       <c r="H27" s="23"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
       <c r="K27" s="23"/>
       <c r="L27" s="23"/>
       <c r="M27" s="23"/>
@@ -1458,7 +1458,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
-      <c r="I29" s="34"/>
+      <c r="I29" s="31"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="7"/>
@@ -1482,7 +1482,7 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="34"/>
+      <c r="I30" s="31"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
@@ -1507,7 +1507,7 @@
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
-      <c r="J31" s="34"/>
+      <c r="J31" s="31"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
@@ -1531,7 +1531,7 @@
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
-      <c r="J32" s="34"/>
+      <c r="J32" s="31"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
@@ -1555,7 +1555,7 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
-      <c r="J33" s="34"/>
+      <c r="J33" s="31"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
@@ -1579,7 +1579,7 @@
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
-      <c r="J34" s="34"/>
+      <c r="J34" s="31"/>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
@@ -1604,7 +1604,7 @@
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
-      <c r="K35" s="34"/>
+      <c r="K35" s="31"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
@@ -1628,7 +1628,7 @@
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
-      <c r="K36" s="34"/>
+      <c r="K36" s="31"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>

</xml_diff>

<commit_message>
opdateret processrapport og realiseret tidsplan for dagens arbejde.
</commit_message>
<xml_diff>
--- a/Assets/Documents/Realiseret_tidsplan.xlsx
+++ b/Assets/Documents/Realiseret_tidsplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\92agg\Desktop\Svendeprøve\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479E0262-1B9D-416C-AEF4-B878ABED3EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0636C9-8DF9-4323-9D53-5FE6376FEE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-7260" windowWidth="16440" windowHeight="28320" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>Projekt startdato:</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Sidernes Verden - Realiseret tidsplan</t>
+  </si>
+  <si>
+    <t>Test af metoder</t>
   </si>
 </sst>
 </file>
@@ -770,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0E67C9-148C-445C-AEDA-6C5F365E02ED}">
   <dimension ref="B1:AB61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,17 +1001,17 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
+      <c r="N11" s="18"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
+      <c r="S11" s="18"/>
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
+      <c r="X11" s="18"/>
       <c r="Z11" s="19"/>
       <c r="AB11" s="4" t="s">
         <v>25</v>
@@ -1190,7 +1193,7 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
+      <c r="K18" s="29"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
@@ -1214,7 +1217,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
+      <c r="K19" s="29"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
@@ -1238,7 +1241,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
+      <c r="K20" s="29"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
@@ -1556,7 +1559,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="31"/>
-      <c r="K33" s="5"/>
+      <c r="K33" s="31"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
@@ -1580,7 +1583,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="31"/>
-      <c r="K34" s="5"/>
+      <c r="K34" s="31"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
@@ -1715,7 +1718,30 @@
       <c r="W39" s="5"/>
       <c r="X39" s="5"/>
     </row>
-    <row r="40" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="5"/>
+      <c r="U40" s="5"/>
+      <c r="V40" s="5"/>
+      <c r="W40" s="5"/>
+      <c r="X40" s="5"/>
+    </row>
     <row r="41" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Opdateret processrapport og realiseret tidsplan med dagens arbejde.
</commit_message>
<xml_diff>
--- a/Assets/Documents/Realiseret_tidsplan.xlsx
+++ b/Assets/Documents/Realiseret_tidsplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\92agg\Desktop\Svendeprøve\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0636C9-8DF9-4323-9D53-5FE6376FEE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD98563E-EFC0-42FB-9BA5-267720D70E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-7260" windowWidth="16440" windowHeight="28320" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0E67C9-148C-445C-AEDA-6C5F365E02ED}">
   <dimension ref="B1:AB61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,7 +1242,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="29"/>
-      <c r="L20" s="5"/>
+      <c r="L20" s="29"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
@@ -1560,7 +1560,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="31"/>
       <c r="K33" s="31"/>
-      <c r="L33" s="5"/>
+      <c r="L33" s="31"/>
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
@@ -1584,7 +1584,7 @@
       <c r="I34" s="5"/>
       <c r="J34" s="31"/>
       <c r="K34" s="31"/>
-      <c r="L34" s="5"/>
+      <c r="L34" s="31"/>
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
@@ -1608,7 +1608,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="31"/>
-      <c r="L35" s="5"/>
+      <c r="L35" s="31"/>
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
@@ -1680,8 +1680,8 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
@@ -1728,8 +1728,8 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="31"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>

</xml_diff>

<commit_message>
Opdateret realiseret tidsplan for dagens arbejde.
</commit_message>
<xml_diff>
--- a/Assets/Documents/Realiseret_tidsplan.xlsx
+++ b/Assets/Documents/Realiseret_tidsplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\92agg\Desktop\Svendeprøve\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD98563E-EFC0-42FB-9BA5-267720D70E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D74934-FCC9-46B2-B8C9-9BEA8D4C54C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
+    <workbookView xWindow="-16320" yWindow="-7260" windowWidth="16440" windowHeight="28320" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -774,7 +774,7 @@
   <dimension ref="B1:AB61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,7 +1681,7 @@
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
       <c r="L38" s="31"/>
-      <c r="M38" s="31"/>
+      <c r="M38" s="5"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
@@ -1729,7 +1729,7 @@
       <c r="J40" s="5"/>
       <c r="K40" s="31"/>
       <c r="L40" s="31"/>
-      <c r="M40" s="31"/>
+      <c r="M40" s="5"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>

</xml_diff>

<commit_message>
opdatering af logbog og realiseret tidsplan for dagens arbejde.
</commit_message>
<xml_diff>
--- a/Assets/Documents/Realiseret_tidsplan.xlsx
+++ b/Assets/Documents/Realiseret_tidsplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\92agg\Desktop\Svendeprøve\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D74934-FCC9-46B2-B8C9-9BEA8D4C54C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA600F1-ABA8-452D-B13F-9BF14D1E48F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-7260" windowWidth="16440" windowHeight="28320" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -774,7 +774,7 @@
   <dimension ref="B1:AB61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,7 +1513,7 @@
       <c r="J31" s="31"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
+      <c r="M31" s="31"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
@@ -1561,7 +1561,7 @@
       <c r="J33" s="31"/>
       <c r="K33" s="31"/>
       <c r="L33" s="31"/>
-      <c r="M33" s="5"/>
+      <c r="M33" s="31"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
@@ -1585,7 +1585,7 @@
       <c r="J34" s="31"/>
       <c r="K34" s="31"/>
       <c r="L34" s="31"/>
-      <c r="M34" s="5"/>
+      <c r="M34" s="31"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
@@ -1681,7 +1681,7 @@
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
       <c r="L38" s="31"/>
-      <c r="M38" s="5"/>
+      <c r="M38" s="31"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
@@ -1729,7 +1729,7 @@
       <c r="J40" s="5"/>
       <c r="K40" s="31"/>
       <c r="L40" s="31"/>
-      <c r="M40" s="5"/>
+      <c r="M40" s="31"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>

</xml_diff>

<commit_message>
opdatering af Procesrapport og Realiseret tidsplan med dagens arbejde.
</commit_message>
<xml_diff>
--- a/Assets/Documents/Realiseret_tidsplan.xlsx
+++ b/Assets/Documents/Realiseret_tidsplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\92agg\Desktop\Svendeprøve\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701C506A-CEFE-427B-8A46-8B6FFF183298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727EC339-6C28-47BC-BE05-F808B8028831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
+    <workbookView xWindow="-16320" yWindow="-7260" windowWidth="16440" windowHeight="28320" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0E67C9-148C-445C-AEDA-6C5F365E02ED}">
   <dimension ref="B1:AB61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,7 +1144,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="29"/>
-      <c r="N16" s="5"/>
+      <c r="N16" s="29"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
@@ -1172,7 +1172,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="29"/>
-      <c r="N17" s="5"/>
+      <c r="N17" s="29"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
@@ -1193,7 +1193,7 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="29"/>
+      <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
@@ -1367,7 +1367,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
+      <c r="N25" s="30"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
@@ -1391,7 +1391,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
+      <c r="N26" s="30"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>

</xml_diff>

<commit_message>
dokumentation for dagens arbejde.
</commit_message>
<xml_diff>
--- a/Assets/Documents/Realiseret_tidsplan.xlsx
+++ b/Assets/Documents/Realiseret_tidsplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\92agg\Desktop\Svendeprøve\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22468D8-EAF2-4DA6-A0ED-8AD49A8D2075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624EAE15-D275-458B-B4FA-1DA2C986407E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-7260" windowWidth="16440" windowHeight="28320" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Projekt startdato:</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Test af metoder</t>
+  </si>
+  <si>
+    <t>Filtrering</t>
   </si>
 </sst>
 </file>
@@ -771,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0E67C9-148C-445C-AEDA-6C5F365E02ED}">
-  <dimension ref="B1:AB61"/>
+  <dimension ref="B1:AB62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q38" sqref="Q38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +897,7 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="13"/>
       <c r="R7" s="13"/>
-      <c r="S7" s="7"/>
+      <c r="S7" s="13"/>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
@@ -922,7 +925,7 @@
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="12"/>
-      <c r="S8" s="5"/>
+      <c r="S8" s="12"/>
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
@@ -1201,7 +1204,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
+      <c r="S18" s="29"/>
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
@@ -1273,7 +1276,7 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
+      <c r="S21" s="29"/>
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
       <c r="V21" s="5"/>
@@ -1297,7 +1300,7 @@
       <c r="P22" s="23"/>
       <c r="Q22" s="23"/>
       <c r="R22" s="23"/>
-      <c r="S22" s="23"/>
+      <c r="S22" s="29"/>
       <c r="T22" s="23"/>
       <c r="U22" s="23"/>
       <c r="V22" s="23"/>
@@ -1372,7 +1375,7 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
+      <c r="S25" s="30"/>
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
@@ -1566,8 +1569,8 @@
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="5"/>
+      <c r="R33" s="31"/>
+      <c r="S33" s="31"/>
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
       <c r="V33" s="5"/>
@@ -1696,7 +1699,7 @@
     </row>
     <row r="39" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
@@ -1708,9 +1711,9 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
-      <c r="P39" s="31"/>
+      <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
+      <c r="R39" s="31"/>
       <c r="S39" s="5"/>
       <c r="T39" s="5"/>
       <c r="U39" s="5"/>
@@ -1720,16 +1723,16 @@
     </row>
     <row r="40" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
-      <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
-      <c r="M40" s="31"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="31"/>
@@ -1742,7 +1745,30 @@
       <c r="W40" s="5"/>
       <c r="X40" s="5"/>
     </row>
-    <row r="41" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="V41" s="5"/>
+      <c r="W41" s="5"/>
+      <c r="X41" s="5"/>
+    </row>
     <row r="42" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1763,6 +1789,7 @@
     <row r="59" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:F2"/>

</xml_diff>

<commit_message>
tilføjelse af bilag for estimeret samt realiseret tidsplan.
</commit_message>
<xml_diff>
--- a/Assets/Documents/Realiseret_tidsplan.xlsx
+++ b/Assets/Documents/Realiseret_tidsplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\92agg\Desktop\Svendeprøve\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624EAE15-D275-458B-B4FA-1DA2C986407E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2E8E06-A462-455C-AF98-8DA2CC34253C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-7260" windowWidth="16440" windowHeight="28320" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -777,7 +777,7 @@
   <dimension ref="B1:AB62"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R39" sqref="R39"/>
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,11 +898,11 @@
       <c r="Q7" s="13"/>
       <c r="R7" s="13"/>
       <c r="S7" s="13"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
       <c r="Z7" s="10"/>
       <c r="AB7" s="4" t="s">
         <v>1</v>
@@ -926,11 +926,11 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="12"/>
       <c r="S8" s="12"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
       <c r="Z8" s="11"/>
       <c r="AB8" s="4" t="s">
         <v>2</v>
@@ -1571,7 +1571,7 @@
       <c r="Q33" s="5"/>
       <c r="R33" s="31"/>
       <c r="S33" s="31"/>
-      <c r="T33" s="5"/>
+      <c r="T33" s="31"/>
       <c r="U33" s="5"/>
       <c r="V33" s="5"/>
       <c r="W33" s="5"/>
@@ -1643,7 +1643,7 @@
       <c r="Q36" s="5"/>
       <c r="R36" s="5"/>
       <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
+      <c r="T36" s="31"/>
       <c r="U36" s="5"/>
       <c r="V36" s="5"/>
       <c r="W36" s="5"/>
@@ -1763,7 +1763,7 @@
       <c r="Q41" s="5"/>
       <c r="R41" s="5"/>
       <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
+      <c r="T41" s="31"/>
       <c r="U41" s="5"/>
       <c r="V41" s="5"/>
       <c r="W41" s="5"/>

</xml_diff>